<commit_message>
initial time series - up to March 25 - simplifying column names
</commit_message>
<xml_diff>
--- a/TompkinsCountyHealthDepartmentCovid19TimeSeries.xlsx
+++ b/TompkinsCountyHealthDepartmentCovid19TimeSeries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\covid-19-TC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1F520C25-A1A1-4672-96E2-BC660111C573}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580A545A-CF9E-4D85-8520-A1D2A3F23CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4673" yWindow="440" windowWidth="19260" windowHeight="12407" xr2:uid="{1C93E160-DEF0-4C5C-99D7-27E91B473392}"/>
+    <workbookView xWindow="5013" yWindow="780" windowWidth="19260" windowHeight="12407" xr2:uid="{1C93E160-DEF0-4C5C-99D7-27E91B473392}"/>
   </bookViews>
   <sheets>
     <sheet name="TompkinsCountyHealthDepartmentC" sheetId="1" r:id="rId1"/>
@@ -39,22 +39,22 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Pending Test Results for COVID-19</t>
+    <t>Pending</t>
   </si>
   <si>
-    <t>Positive Test Results</t>
+    <t>Positive</t>
   </si>
   <si>
-    <t>Negative Test Results</t>
+    <t>Negative</t>
   </si>
   <si>
-    <t>Total Tested</t>
+    <t>Total_tested</t>
   </si>
   <si>
-    <t>In Quarantine and Monitored by TCHD</t>
+    <t>In_quarantine</t>
   </si>
   <si>
-    <t>Released from Quarantine</t>
+    <t>Released_quarantine</t>
   </si>
 </sst>
 </file>
@@ -62,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -109,13 +109,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,7 +433,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -444,10 +444,10 @@
     <col min="4" max="4" width="14.05859375" customWidth="1"/>
     <col min="5" max="5" width="14.17578125" customWidth="1"/>
     <col min="6" max="6" width="16.41015625" customWidth="1"/>
-    <col min="7" max="7" width="16.76171875" customWidth="1"/>
+    <col min="7" max="7" width="19.64453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
initial time series - up to March 25 - simplifying column names - adding day number
</commit_message>
<xml_diff>
--- a/TompkinsCountyHealthDepartmentCovid19TimeSeries.xlsx
+++ b/TompkinsCountyHealthDepartmentCovid19TimeSeries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\covid-19-TC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580A545A-CF9E-4D85-8520-A1D2A3F23CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D0D069-64D1-4F00-B4D8-52642C0FF7AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5013" yWindow="780" windowWidth="19260" windowHeight="12407" xr2:uid="{1C93E160-DEF0-4C5C-99D7-27E91B473392}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="TompkinsCountyHealthDepartmentC" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_Hlk35725696" localSheetId="0">TompkinsCountyHealthDepartmentC!$A$1</definedName>
+    <definedName name="_Hlk35725696" localSheetId="0">TompkinsCountyHealthDepartmentC!$B$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Released_quarantine</t>
+  </si>
+  <si>
+    <t>Day</t>
   </si>
 </sst>
 </file>
@@ -101,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -116,6 +119,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,256 +434,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0983A088-8A80-47BD-A01C-EDB7EE767BA4}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="19.87890625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="18.9375" customWidth="1"/>
-    <col min="3" max="3" width="14.29296875" customWidth="1"/>
-    <col min="4" max="4" width="14.05859375" customWidth="1"/>
-    <col min="5" max="5" width="14.17578125" customWidth="1"/>
-    <col min="6" max="6" width="16.41015625" customWidth="1"/>
-    <col min="7" max="7" width="19.64453125" customWidth="1"/>
+    <col min="2" max="2" width="19.87890625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.9375" customWidth="1"/>
+    <col min="4" max="4" width="14.29296875" customWidth="1"/>
+    <col min="5" max="5" width="14.05859375" customWidth="1"/>
+    <col min="6" max="6" width="14.17578125" customWidth="1"/>
+    <col min="7" max="7" width="16.41015625" customWidth="1"/>
+    <col min="8" max="8" width="19.64453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A2" s="4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
         <v>43907</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C2" s="2">
         <v>69</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>3</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>35</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>107</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>82</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A3" s="4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
         <v>43908</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="2">
         <v>93</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>6</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>46</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>146</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>86</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A4" s="4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <f t="shared" ref="A4:A10" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
         <v>43909</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4" s="2">
         <v>224</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>6</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>49</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>279</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>293</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A5" s="4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
         <v>43910</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C5" s="2">
         <v>280</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>11</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>88</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>379</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>515</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A6" s="4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
         <v>43911</v>
       </c>
-      <c r="B6" s="2">
+      <c r="C6" s="2">
         <v>302</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>12</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>135</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>449</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>418</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A7" s="4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
         <v>43912</v>
       </c>
-      <c r="B7" s="2">
+      <c r="C7" s="2">
         <v>276</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>15</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>160</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>451</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>397</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A8" s="4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
         <v>43913</v>
       </c>
-      <c r="B8" s="2">
+      <c r="C8" s="2">
         <v>251</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>16</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>325</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>592</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>244</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>344</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A9" s="4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
         <v>43914</v>
       </c>
-      <c r="B9" s="2">
+      <c r="C9" s="2">
         <v>218</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>18</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>430</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>666</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>326</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>441</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A10" s="4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
         <v>43915</v>
       </c>
-      <c r="B10" s="2">
+      <c r="C10" s="2">
         <v>236</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>23</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>472</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>731</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>351</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>484</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G10">
-    <sortCondition ref="A2:A10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H10">
+    <sortCondition ref="B2:B10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Merged Data for world and New York State and Tompkins
</commit_message>
<xml_diff>
--- a/TompkinsCountyHealthDepartmentCovid19TimeSeries.xlsx
+++ b/TompkinsCountyHealthDepartmentCovid19TimeSeries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\covid-19-TC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D0D069-64D1-4F00-B4D8-52642C0FF7AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E98D57-6B11-460B-81ED-7C49D5A70D2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5013" yWindow="780" windowWidth="19260" windowHeight="12407" xr2:uid="{1C93E160-DEF0-4C5C-99D7-27E91B473392}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Day</t>
+  </si>
+  <si>
+    <t>Deaths</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -120,6 +123,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,9 +440,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0983A088-8A80-47BD-A01C-EDB7EE767BA4}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
@@ -449,7 +457,7 @@
     <col min="8" max="8" width="19.64453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -474,8 +482,11 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -500,8 +511,11 @@
       <c r="H2" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -527,8 +541,11 @@
       <c r="H3" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -554,8 +571,11 @@
       <c r="H4" s="2">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -581,8 +601,11 @@
       <c r="H5" s="2">
         <v>153</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -608,8 +631,11 @@
       <c r="H6" s="2">
         <v>206</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -635,8 +661,11 @@
       <c r="H7" s="2">
         <v>235</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -662,8 +691,11 @@
       <c r="H8" s="2">
         <v>344</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -689,8 +721,11 @@
       <c r="H9" s="2">
         <v>441</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -715,6 +750,9 @@
       </c>
       <c r="H10" s="2">
         <v>484</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Tompkins for March 26
</commit_message>
<xml_diff>
--- a/TompkinsCountyHealthDepartmentCovid19TimeSeries.xlsx
+++ b/TompkinsCountyHealthDepartmentCovid19TimeSeries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\covid-19-TC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E98D57-6B11-460B-81ED-7C49D5A70D2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36AE7DC-99D8-4CC2-860F-9C3819A1A30E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5013" yWindow="780" windowWidth="19260" windowHeight="12407" xr2:uid="{1C93E160-DEF0-4C5C-99D7-27E91B473392}"/>
+    <workbookView xWindow="7373" yWindow="1240" windowWidth="16300" windowHeight="12407" xr2:uid="{1C93E160-DEF0-4C5C-99D7-27E91B473392}"/>
   </bookViews>
   <sheets>
     <sheet name="TompkinsCountyHealthDepartmentC" sheetId="1" r:id="rId1"/>
@@ -440,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0983A088-8A80-47BD-A01C-EDB7EE767BA4}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -755,6 +755,36 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <f>B10+1</f>
+        <v>43916</v>
+      </c>
+      <c r="C11" s="7">
+        <v>462</v>
+      </c>
+      <c r="D11" s="7">
+        <v>32</v>
+      </c>
+      <c r="E11" s="7">
+        <v>515</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1009</v>
+      </c>
+      <c r="G11" s="7">
+        <v>354</v>
+      </c>
+      <c r="H11" s="7">
+        <v>526</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H10">
     <sortCondition ref="B2:B10"/>

</xml_diff>

<commit_message>
update to include pending - now available again.
</commit_message>
<xml_diff>
--- a/TompkinsCountyHealthDepartmentCovid19TimeSeries.xlsx
+++ b/TompkinsCountyHealthDepartmentCovid19TimeSeries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\covid-19-TC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A598A64F-63D0-4B99-BC0A-8296E199E665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4959554-EA56-4141-AC03-9C804F52AF8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4953" yWindow="913" windowWidth="15934" windowHeight="12407" xr2:uid="{1C93E160-DEF0-4C5C-99D7-27E91B473392}"/>
   </bookViews>
@@ -457,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0983A088-8A80-47BD-A01C-EDB7EE767BA4}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -895,7 +895,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5">
-        <f>B10+1</f>
+        <f t="shared" ref="B11:B16" si="1">B10+1</f>
         <v>43916</v>
       </c>
       <c r="C11" s="7">
@@ -937,7 +937,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="5">
-        <f>B11+1</f>
+        <f t="shared" si="1"/>
         <v>43917</v>
       </c>
       <c r="C12" s="7">
@@ -980,7 +980,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5">
-        <f>B12+1</f>
+        <f t="shared" si="1"/>
         <v>43918</v>
       </c>
       <c r="C13" t="e">
@@ -1023,7 +1023,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="5">
-        <f>B13+1</f>
+        <f t="shared" si="1"/>
         <v>43919</v>
       </c>
       <c r="C14" t="e">
@@ -1066,7 +1066,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5">
-        <f>B14+1</f>
+        <f t="shared" si="1"/>
         <v>43920</v>
       </c>
       <c r="C15" t="e">
@@ -1109,11 +1109,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="5">
-        <f>B15+1</f>
+        <f t="shared" si="1"/>
         <v>43921</v>
       </c>
-      <c r="C16" t="e">
-        <v>#N/A</v>
+      <c r="C16">
+        <v>242</v>
       </c>
       <c r="D16" s="7">
         <v>76</v>

</xml_diff>